<commit_message>
new improved limits method
</commit_message>
<xml_diff>
--- a/Parameter.xlsx
+++ b/Parameter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim Schell\Documents\GitHub\Limits-to-Growth-Masterprojekt-TH-Koeln-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE843998-5CE4-4158-83EE-20B5703D4BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3B779E-94D7-406C-BE74-572BB1303D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3F5EE684-BD36-5A47-B2A5-759BDA655248}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3F5EE684-BD36-5A47-B2A5-759BDA655248}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -468,7 +468,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B2:B17"/>
+      <selection activeCell="B9" sqref="B5:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>